<commit_message>
updated code with date modification
</commit_message>
<xml_diff>
--- a/data/Production_Filled_April.xlsx
+++ b/data/Production_Filled_April.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\Filter_form\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\test\Filter_form\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -220,6 +220,9 @@
     <t>Spinning Prod.</t>
   </si>
   <si>
+    <t xml:space="preserve"> TWISTING PROD</t>
+  </si>
+  <si>
     <t xml:space="preserve">TWISTING PACKED </t>
   </si>
   <si>
@@ -305,9 +308,6 @@
   </si>
   <si>
     <t>SOIL SAVAR INCREASE / DECREASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TWISTING PRODUCTION</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,94 +1403,94 @@
         <v>4</v>
       </c>
       <c r="F1" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB1" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC1" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD1" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE1" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF1" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG1" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI1" s="49" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z1" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA1" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB1" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF1" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG1" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH1" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="AI1" s="49" t="s">
-        <v>92</v>
       </c>
       <c r="AJ1" s="50" t="s">
         <v>3</v>
@@ -5142,7 +5142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Z57" sqref="Z57"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fully_Modified for Product wise list
</commit_message>
<xml_diff>
--- a/data/Production_Filled_April.xlsx
+++ b/data/Production_Filled_April.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\test\Filter_form\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\Filter_form\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Total_Salable_Prod" sheetId="2" r:id="rId2"/>
     <sheet name="Product_Wise" sheetId="3" r:id="rId3"/>
+    <sheet name="Spinning_Prod" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Twisting_Prod" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Weaving_Prod" sheetId="6" r:id="rId6"/>
+    <sheet name="Spool_Winding_Stock" sheetId="7" r:id="rId7"/>
+    <sheet name="Cop_Winding_Stock" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>DATE</t>
   </si>
@@ -315,7 +320,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +367,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -555,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -659,6 +687,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1774,7 +1809,7 @@
       </c>
       <c r="N4" s="45"/>
       <c r="O4" s="45">
-        <f t="shared" ref="O3:O27" si="4">+M4-M3</f>
+        <f t="shared" ref="O4:O27" si="4">+M4-M3</f>
         <v>0</v>
       </c>
       <c r="P4" s="45">
@@ -5132,8 +5167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:AA53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10056,4 +10091,3501 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="59" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58">
+        <v>45748</v>
+      </c>
+      <c r="C1" s="58">
+        <v>45749</v>
+      </c>
+      <c r="D1" s="58">
+        <v>45750</v>
+      </c>
+      <c r="E1" s="58">
+        <v>45752</v>
+      </c>
+      <c r="F1" s="58">
+        <v>45753</v>
+      </c>
+      <c r="G1" s="58">
+        <v>45754</v>
+      </c>
+      <c r="H1" s="58">
+        <v>45755</v>
+      </c>
+      <c r="I1" s="58">
+        <v>45756</v>
+      </c>
+      <c r="J1" s="58">
+        <v>45757</v>
+      </c>
+      <c r="K1" s="58">
+        <v>45759</v>
+      </c>
+      <c r="L1" s="58">
+        <v>45760</v>
+      </c>
+      <c r="M1" s="58">
+        <v>45761</v>
+      </c>
+      <c r="N1" s="58">
+        <v>45762</v>
+      </c>
+      <c r="O1" s="58">
+        <v>45763</v>
+      </c>
+      <c r="P1" s="58">
+        <v>45764</v>
+      </c>
+      <c r="Q1" s="58">
+        <v>45766</v>
+      </c>
+      <c r="R1" s="58">
+        <v>45767</v>
+      </c>
+      <c r="S1" s="58">
+        <v>45768</v>
+      </c>
+      <c r="T1" s="58">
+        <v>45769</v>
+      </c>
+      <c r="U1" s="58">
+        <v>45770</v>
+      </c>
+      <c r="V1" s="58">
+        <v>45771</v>
+      </c>
+      <c r="W1" s="58">
+        <v>45773</v>
+      </c>
+      <c r="X1" s="58">
+        <v>45774</v>
+      </c>
+      <c r="Y1" s="58">
+        <v>45775</v>
+      </c>
+      <c r="Z1" s="58">
+        <v>45776</v>
+      </c>
+      <c r="AA1" s="58">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
+        <v>126.5</v>
+      </c>
+      <c r="C2" s="24">
+        <v>130</v>
+      </c>
+      <c r="D2" s="23">
+        <v>132</v>
+      </c>
+      <c r="E2" s="23">
+        <v>131</v>
+      </c>
+      <c r="F2" s="23">
+        <v>95</v>
+      </c>
+      <c r="G2" s="23">
+        <v>131</v>
+      </c>
+      <c r="H2" s="23">
+        <v>128</v>
+      </c>
+      <c r="I2" s="24">
+        <v>132.5</v>
+      </c>
+      <c r="J2" s="24">
+        <v>130</v>
+      </c>
+      <c r="K2" s="24">
+        <v>131</v>
+      </c>
+      <c r="L2" s="24">
+        <v>130</v>
+      </c>
+      <c r="M2" s="24">
+        <v>130</v>
+      </c>
+      <c r="N2" s="24">
+        <v>130</v>
+      </c>
+      <c r="O2" s="24">
+        <v>131</v>
+      </c>
+      <c r="P2" s="24">
+        <v>133</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>129</v>
+      </c>
+      <c r="R2" s="24">
+        <v>129</v>
+      </c>
+      <c r="S2" s="24">
+        <v>130</v>
+      </c>
+      <c r="T2" s="24">
+        <v>130</v>
+      </c>
+      <c r="U2" s="24">
+        <v>130</v>
+      </c>
+      <c r="V2" s="24">
+        <v>131</v>
+      </c>
+      <c r="W2" s="24">
+        <v>129</v>
+      </c>
+      <c r="X2" s="24">
+        <v>129</v>
+      </c>
+      <c r="Y2" s="24">
+        <v>129</v>
+      </c>
+      <c r="Z2" s="24">
+        <v>130</v>
+      </c>
+      <c r="AA2" s="24">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.476</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.16</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2.82</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.8050000000000002</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.86</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2.2389999999999999</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3.04</v>
+      </c>
+      <c r="N3" s="3">
+        <v>3.0379999999999998</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="P3" s="3">
+        <v>3.06</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>3.02</v>
+      </c>
+      <c r="R3" s="3">
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="S3" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="T3" s="3">
+        <v>3.125</v>
+      </c>
+      <c r="U3" s="3">
+        <v>2.8279999999999998</v>
+      </c>
+      <c r="V3" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2.2719999999999998</v>
+      </c>
+      <c r="X3" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>2.61</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>2.71</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.36</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3">
+        <v>16.695</v>
+      </c>
+      <c r="C6" s="3">
+        <v>17.234999999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>17.097999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>17.25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>14.242000000000001</v>
+      </c>
+      <c r="G6" s="3">
+        <v>16.538</v>
+      </c>
+      <c r="H6" s="3">
+        <v>16.475000000000001</v>
+      </c>
+      <c r="I6" s="3">
+        <v>16.055</v>
+      </c>
+      <c r="J6" s="3">
+        <v>16</v>
+      </c>
+      <c r="K6" s="3">
+        <v>16.675999999999998</v>
+      </c>
+      <c r="L6" s="3">
+        <v>15.98</v>
+      </c>
+      <c r="M6" s="3">
+        <v>14.583</v>
+      </c>
+      <c r="N6" s="3">
+        <v>14.305999999999999</v>
+      </c>
+      <c r="O6" s="3">
+        <v>14.925000000000001</v>
+      </c>
+      <c r="P6" s="3">
+        <v>13.625999999999999</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>14.273999999999999</v>
+      </c>
+      <c r="R6" s="3">
+        <v>14.478</v>
+      </c>
+      <c r="S6" s="3">
+        <v>14.446</v>
+      </c>
+      <c r="T6" s="3">
+        <v>14.680999999999999</v>
+      </c>
+      <c r="U6" s="3">
+        <v>14.731999999999999</v>
+      </c>
+      <c r="V6" s="3">
+        <v>14.811999999999999</v>
+      </c>
+      <c r="W6" s="3">
+        <v>14.45</v>
+      </c>
+      <c r="X6" s="3">
+        <v>14.449</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>14.432</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>13.816000000000001</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>14.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.915</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.63</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.845</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.845</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1.9259999999999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.92</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.8380000000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.875</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.9079999999999999</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3.758</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3.8959999999999999</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4.42</v>
+      </c>
+      <c r="P7" s="3">
+        <v>4.8639999999999999</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="R7" s="3">
+        <v>4.9450000000000003</v>
+      </c>
+      <c r="S7" s="3">
+        <v>4.9580000000000002</v>
+      </c>
+      <c r="T7" s="3">
+        <v>4.88</v>
+      </c>
+      <c r="U7" s="3">
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="V7" s="3">
+        <v>4.867</v>
+      </c>
+      <c r="W7" s="3">
+        <v>5.0250000000000004</v>
+      </c>
+      <c r="X7" s="3">
+        <v>4.95</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>4.9450000000000003</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>4.8600000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12.002000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12.696</v>
+      </c>
+      <c r="D8" s="3">
+        <v>12.54</v>
+      </c>
+      <c r="E8" s="3">
+        <v>12.625</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="G8" s="3">
+        <v>12.67</v>
+      </c>
+      <c r="H8" s="3">
+        <v>12.91</v>
+      </c>
+      <c r="I8" s="3">
+        <v>12.71</v>
+      </c>
+      <c r="J8" s="3">
+        <v>12.79</v>
+      </c>
+      <c r="K8" s="3">
+        <v>11.935</v>
+      </c>
+      <c r="L8" s="3">
+        <v>12.75</v>
+      </c>
+      <c r="M8" s="3">
+        <v>12.476000000000001</v>
+      </c>
+      <c r="N8" s="3">
+        <v>12.952999999999999</v>
+      </c>
+      <c r="O8" s="3">
+        <v>11.882999999999999</v>
+      </c>
+      <c r="P8" s="3">
+        <v>12.984</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>11.683999999999999</v>
+      </c>
+      <c r="R8" s="3">
+        <v>11.759</v>
+      </c>
+      <c r="S8" s="3">
+        <v>12.218</v>
+      </c>
+      <c r="T8" s="3">
+        <v>12.037000000000001</v>
+      </c>
+      <c r="U8" s="3">
+        <v>12.375</v>
+      </c>
+      <c r="V8" s="3">
+        <v>12.617000000000001</v>
+      </c>
+      <c r="W8" s="3">
+        <v>12.69</v>
+      </c>
+      <c r="X8" s="3">
+        <v>12.757999999999999</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>12.728999999999999</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>13.13</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1.42</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1.42</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="R9" s="3">
+        <v>1.4470000000000001</v>
+      </c>
+      <c r="S9" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="T9" s="3">
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="V9" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1.478</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>1.518</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="S10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="27" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="59" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58">
+        <v>45748</v>
+      </c>
+      <c r="C1" s="58">
+        <v>45749</v>
+      </c>
+      <c r="D1" s="58">
+        <v>45750</v>
+      </c>
+      <c r="E1" s="58">
+        <v>45752</v>
+      </c>
+      <c r="F1" s="58">
+        <v>45753</v>
+      </c>
+      <c r="G1" s="58">
+        <v>45754</v>
+      </c>
+      <c r="H1" s="58">
+        <v>45755</v>
+      </c>
+      <c r="I1" s="58">
+        <v>45756</v>
+      </c>
+      <c r="J1" s="58">
+        <v>45757</v>
+      </c>
+      <c r="K1" s="58">
+        <v>45759</v>
+      </c>
+      <c r="L1" s="58">
+        <v>45760</v>
+      </c>
+      <c r="M1" s="58">
+        <v>45761</v>
+      </c>
+      <c r="N1" s="58">
+        <v>45762</v>
+      </c>
+      <c r="O1" s="58">
+        <v>45763</v>
+      </c>
+      <c r="P1" s="58">
+        <v>45764</v>
+      </c>
+      <c r="Q1" s="58">
+        <v>45766</v>
+      </c>
+      <c r="R1" s="58">
+        <v>45767</v>
+      </c>
+      <c r="S1" s="58">
+        <v>45768</v>
+      </c>
+      <c r="T1" s="58">
+        <v>45769</v>
+      </c>
+      <c r="U1" s="58">
+        <v>45770</v>
+      </c>
+      <c r="V1" s="58">
+        <v>45771</v>
+      </c>
+      <c r="W1" s="58">
+        <v>45773</v>
+      </c>
+      <c r="X1" s="58">
+        <v>45774</v>
+      </c>
+      <c r="Y1" s="58">
+        <v>45775</v>
+      </c>
+      <c r="Z1" s="58">
+        <v>45776</v>
+      </c>
+      <c r="AA1" s="58">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.749</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="V2" s="4">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="W2" s="4">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="X2" s="4">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>1.006</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="27" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58">
+        <v>45748</v>
+      </c>
+      <c r="C1" s="58">
+        <v>45749</v>
+      </c>
+      <c r="D1" s="58">
+        <v>45750</v>
+      </c>
+      <c r="E1" s="58">
+        <v>45752</v>
+      </c>
+      <c r="F1" s="58">
+        <v>45753</v>
+      </c>
+      <c r="G1" s="58">
+        <v>45754</v>
+      </c>
+      <c r="H1" s="58">
+        <v>45755</v>
+      </c>
+      <c r="I1" s="58">
+        <v>45756</v>
+      </c>
+      <c r="J1" s="58">
+        <v>45757</v>
+      </c>
+      <c r="K1" s="58">
+        <v>45759</v>
+      </c>
+      <c r="L1" s="58">
+        <v>45760</v>
+      </c>
+      <c r="M1" s="58">
+        <v>45761</v>
+      </c>
+      <c r="N1" s="58">
+        <v>45762</v>
+      </c>
+      <c r="O1" s="58">
+        <v>45763</v>
+      </c>
+      <c r="P1" s="58">
+        <v>45764</v>
+      </c>
+      <c r="Q1" s="58">
+        <v>45766</v>
+      </c>
+      <c r="R1" s="58">
+        <v>45767</v>
+      </c>
+      <c r="S1" s="58">
+        <v>45768</v>
+      </c>
+      <c r="T1" s="58">
+        <v>45769</v>
+      </c>
+      <c r="U1" s="58">
+        <v>45770</v>
+      </c>
+      <c r="V1" s="58">
+        <v>45771</v>
+      </c>
+      <c r="W1" s="58">
+        <v>45773</v>
+      </c>
+      <c r="X1" s="58">
+        <v>45774</v>
+      </c>
+      <c r="Y1" s="58">
+        <v>45775</v>
+      </c>
+      <c r="Z1" s="58">
+        <v>45776</v>
+      </c>
+      <c r="AA1" s="58">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.875</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.9609999999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.738</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2.6059999999999999</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.726</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2.5209999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2.6389999999999998</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2.6419999999999999</v>
+      </c>
+      <c r="O2" s="3">
+        <v>2.871</v>
+      </c>
+      <c r="P2" s="3">
+        <v>2.871</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>2.8029999999999999</v>
+      </c>
+      <c r="R2" s="3">
+        <v>2.7229999999999999</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2.8050000000000002</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="V2" s="3">
+        <v>2.2210000000000001</v>
+      </c>
+      <c r="W2" s="3">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="X2" s="3">
+        <v>3.4689999999999999</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>2.7149999999999999</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>2.3159999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3">
+        <v>23.984999999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <v>24.805</v>
+      </c>
+      <c r="D3" s="3">
+        <v>22.077999999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.128</v>
+      </c>
+      <c r="F3" s="3">
+        <v>21.26</v>
+      </c>
+      <c r="G3" s="3">
+        <v>24.594000000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <v>24.483000000000001</v>
+      </c>
+      <c r="I3" s="3">
+        <v>24.327999999999999</v>
+      </c>
+      <c r="J3" s="3">
+        <v>26.141999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="L3" s="6">
+        <v>24.167999999999999</v>
+      </c>
+      <c r="M3" s="3">
+        <v>25.867000000000001</v>
+      </c>
+      <c r="N3" s="3">
+        <v>24.114000000000001</v>
+      </c>
+      <c r="O3" s="3">
+        <v>21.960999999999999</v>
+      </c>
+      <c r="P3" s="3">
+        <v>21.16</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>25.100999999999999</v>
+      </c>
+      <c r="R3" s="3">
+        <v>24.094999999999999</v>
+      </c>
+      <c r="S3" s="3">
+        <v>24.675999999999998</v>
+      </c>
+      <c r="T3" s="3">
+        <v>24.710999999999999</v>
+      </c>
+      <c r="U3" s="3">
+        <v>24.475000000000001</v>
+      </c>
+      <c r="V3" s="3">
+        <v>25.216999999999999</v>
+      </c>
+      <c r="W3" s="3">
+        <v>25.370999999999999</v>
+      </c>
+      <c r="X3" s="3">
+        <v>24.001000000000001</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>24.068999999999999</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>25.01</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>22.672999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.8439999999999999</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.6040000000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.617</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3.0840000000000001</v>
+      </c>
+      <c r="L4" s="6">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="M4" s="3">
+        <v>3.0840000000000001</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2.8439999999999999</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2.9769999999999999</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3.0840000000000001</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="R4" s="3">
+        <v>2.9769999999999999</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="T4" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="U4" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="V4" s="3">
+        <v>2.8570000000000002</v>
+      </c>
+      <c r="W4" s="3">
+        <v>3.0840000000000001</v>
+      </c>
+      <c r="X4" s="3">
+        <v>2.8570000000000002</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>2.964</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>3.2040000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.371</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.374</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.374</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.253</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.318</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.317</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0.34100000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.123</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.151</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.123</v>
+      </c>
+      <c r="P6" s="3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="R6" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="S6" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.115</v>
+      </c>
+      <c r="U6" s="3">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.121</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0.151</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0.161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AA12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="27" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58">
+        <v>45748</v>
+      </c>
+      <c r="C1" s="58">
+        <v>45749</v>
+      </c>
+      <c r="D1" s="58">
+        <v>45750</v>
+      </c>
+      <c r="E1" s="58">
+        <v>45752</v>
+      </c>
+      <c r="F1" s="58">
+        <v>45753</v>
+      </c>
+      <c r="G1" s="58">
+        <v>45754</v>
+      </c>
+      <c r="H1" s="58">
+        <v>45755</v>
+      </c>
+      <c r="I1" s="58">
+        <v>45756</v>
+      </c>
+      <c r="J1" s="58">
+        <v>45757</v>
+      </c>
+      <c r="K1" s="58">
+        <v>45759</v>
+      </c>
+      <c r="L1" s="58">
+        <v>45760</v>
+      </c>
+      <c r="M1" s="58">
+        <v>45761</v>
+      </c>
+      <c r="N1" s="58">
+        <v>45762</v>
+      </c>
+      <c r="O1" s="58">
+        <v>45763</v>
+      </c>
+      <c r="P1" s="58">
+        <v>45764</v>
+      </c>
+      <c r="Q1" s="58">
+        <v>45766</v>
+      </c>
+      <c r="R1" s="58">
+        <v>45767</v>
+      </c>
+      <c r="S1" s="58">
+        <v>45768</v>
+      </c>
+      <c r="T1" s="58">
+        <v>45769</v>
+      </c>
+      <c r="U1" s="58">
+        <v>45770</v>
+      </c>
+      <c r="V1" s="58">
+        <v>45771</v>
+      </c>
+      <c r="W1" s="58">
+        <v>45773</v>
+      </c>
+      <c r="X1" s="58">
+        <v>45774</v>
+      </c>
+      <c r="Y1" s="58">
+        <v>45775</v>
+      </c>
+      <c r="Z1" s="58">
+        <v>45776</v>
+      </c>
+      <c r="AA1" s="58">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.25</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.625</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1.71</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="R2" s="3">
+        <v>2</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V2" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="W2" s="3">
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="X2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6.95</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7.45</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="I3" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="J3" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="N3" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="O3" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="P3" s="3">
+        <v>6.86</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="R3" s="3">
+        <v>7</v>
+      </c>
+      <c r="S3" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="T3" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="U3" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="V3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="W3" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="X3" s="3">
+        <v>8.75</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>10.25</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.745</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3">
+        <v>12.75</v>
+      </c>
+      <c r="F5" s="3">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3">
+        <v>13.75</v>
+      </c>
+      <c r="H5" s="3">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3">
+        <v>15.75</v>
+      </c>
+      <c r="J5" s="3">
+        <v>17</v>
+      </c>
+      <c r="K5" s="3">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="N5" s="3">
+        <v>19</v>
+      </c>
+      <c r="O5" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="P5" s="3">
+        <v>18.45</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>18</v>
+      </c>
+      <c r="R5" s="3">
+        <v>18</v>
+      </c>
+      <c r="S5" s="3">
+        <v>18</v>
+      </c>
+      <c r="T5" s="3">
+        <v>18</v>
+      </c>
+      <c r="U5" s="3">
+        <v>20</v>
+      </c>
+      <c r="V5" s="3">
+        <v>20.25</v>
+      </c>
+      <c r="W5" s="3">
+        <v>20.25</v>
+      </c>
+      <c r="X5" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3">
+        <v>13.75</v>
+      </c>
+      <c r="C6" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>21.5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3">
+        <v>24</v>
+      </c>
+      <c r="K6" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="L6" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="O6" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="R6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="S6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="T6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="U6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="V6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="W6" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="X6" s="3">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.875</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5.78</v>
+      </c>
+      <c r="M7" s="3">
+        <v>9.5380000000000003</v>
+      </c>
+      <c r="N7" s="3">
+        <v>13.436999999999999</v>
+      </c>
+      <c r="O7" s="3">
+        <v>17.856999999999999</v>
+      </c>
+      <c r="P7" s="3">
+        <v>22.721</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>27.571000000000002</v>
+      </c>
+      <c r="R7" s="3">
+        <v>20.367999999999999</v>
+      </c>
+      <c r="S7" s="3">
+        <v>25.326000000000001</v>
+      </c>
+      <c r="T7" s="3">
+        <v>29.206</v>
+      </c>
+      <c r="U7" s="3">
+        <v>34.220999999999997</v>
+      </c>
+      <c r="V7" s="3">
+        <v>28.163</v>
+      </c>
+      <c r="W7" s="3">
+        <v>33.188000000000002</v>
+      </c>
+      <c r="X7" s="3">
+        <v>38.137999999999998</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>43.113999999999997</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>72.135999999999996</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>76.995999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.375</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>7.625</v>
+      </c>
+      <c r="I8" s="25">
+        <v>7.625</v>
+      </c>
+      <c r="J8" s="3">
+        <v>7.625</v>
+      </c>
+      <c r="K8" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="L8" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="M8" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="N8" s="3">
+        <v>7.9749999999999996</v>
+      </c>
+      <c r="O8" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P8" s="3">
+        <v>7.93</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="R8" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="S8" s="3">
+        <v>8</v>
+      </c>
+      <c r="T8" s="3">
+        <v>8</v>
+      </c>
+      <c r="U8" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="V8" s="3">
+        <v>7.65</v>
+      </c>
+      <c r="W8" s="3">
+        <v>8.125</v>
+      </c>
+      <c r="X8" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>8.25</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>8.65</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4.25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.625</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4.25</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4.625</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.375</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>7.625</v>
+      </c>
+      <c r="I10" s="3">
+        <v>7.625</v>
+      </c>
+      <c r="J10" s="3">
+        <v>7.625</v>
+      </c>
+      <c r="K10" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="L10" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="M10" s="3">
+        <v>7.375</v>
+      </c>
+      <c r="N10" s="3">
+        <v>7.9749999999999996</v>
+      </c>
+      <c r="O10" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P10" s="3">
+        <v>7.93</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="R10" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="S10" s="3">
+        <v>8</v>
+      </c>
+      <c r="T10" s="3">
+        <v>8</v>
+      </c>
+      <c r="U10" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="V10" s="3">
+        <v>7.65</v>
+      </c>
+      <c r="W10" s="3">
+        <v>8.125</v>
+      </c>
+      <c r="X10" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>8.25</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>8.65</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.48</v>
+      </c>
+      <c r="M11" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N11" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="O11" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="P11" s="3">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>2.09</v>
+      </c>
+      <c r="R11" s="3">
+        <v>2</v>
+      </c>
+      <c r="S11" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="T11" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="U11" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="V11" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="W11" s="3">
+        <v>2</v>
+      </c>
+      <c r="X11" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2</v>
+      </c>
+      <c r="P12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2</v>
+      </c>
+      <c r="R12" s="3">
+        <v>2</v>
+      </c>
+      <c r="S12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="T12" s="3">
+        <v>2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
+        <v>2</v>
+      </c>
+      <c r="W12" s="3">
+        <v>2</v>
+      </c>
+      <c r="X12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA11"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="27" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58">
+        <v>45748</v>
+      </c>
+      <c r="C1" s="58">
+        <v>45749</v>
+      </c>
+      <c r="D1" s="58">
+        <v>45750</v>
+      </c>
+      <c r="E1" s="58">
+        <v>45752</v>
+      </c>
+      <c r="F1" s="58">
+        <v>45753</v>
+      </c>
+      <c r="G1" s="58">
+        <v>45754</v>
+      </c>
+      <c r="H1" s="58">
+        <v>45755</v>
+      </c>
+      <c r="I1" s="58">
+        <v>45756</v>
+      </c>
+      <c r="J1" s="58">
+        <v>45757</v>
+      </c>
+      <c r="K1" s="58">
+        <v>45759</v>
+      </c>
+      <c r="L1" s="58">
+        <v>45760</v>
+      </c>
+      <c r="M1" s="58">
+        <v>45761</v>
+      </c>
+      <c r="N1" s="58">
+        <v>45762</v>
+      </c>
+      <c r="O1" s="58">
+        <v>45763</v>
+      </c>
+      <c r="P1" s="58">
+        <v>45764</v>
+      </c>
+      <c r="Q1" s="58">
+        <v>45766</v>
+      </c>
+      <c r="R1" s="58">
+        <v>45767</v>
+      </c>
+      <c r="S1" s="58">
+        <v>45768</v>
+      </c>
+      <c r="T1" s="58">
+        <v>45769</v>
+      </c>
+      <c r="U1" s="58">
+        <v>45770</v>
+      </c>
+      <c r="V1" s="58">
+        <v>45771</v>
+      </c>
+      <c r="W1" s="58">
+        <v>45773</v>
+      </c>
+      <c r="X1" s="58">
+        <v>45774</v>
+      </c>
+      <c r="Y1" s="58">
+        <v>45775</v>
+      </c>
+      <c r="Z1" s="58">
+        <v>45776</v>
+      </c>
+      <c r="AA1" s="58">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3.84</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.7349999999999999</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.57</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.375</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3.15</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.375</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="I2" s="3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="J2" s="3">
+        <v>4.125</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4.1849999999999996</v>
+      </c>
+      <c r="L2" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M2" s="3">
+        <v>4.1849999999999996</v>
+      </c>
+      <c r="N2" s="3">
+        <v>4.95</v>
+      </c>
+      <c r="O2" s="3">
+        <v>6.2249999999999996</v>
+      </c>
+      <c r="P2" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>7.05</v>
+      </c>
+      <c r="R2" s="3">
+        <v>7.17</v>
+      </c>
+      <c r="S2" s="3">
+        <v>6.9749999999999996</v>
+      </c>
+      <c r="T2" s="3">
+        <v>7.05</v>
+      </c>
+      <c r="U2" s="3">
+        <v>7.2750000000000004</v>
+      </c>
+      <c r="V2" s="3">
+        <v>7.4249999999999998</v>
+      </c>
+      <c r="W2" s="3">
+        <v>7.4850000000000003</v>
+      </c>
+      <c r="X2" s="3">
+        <v>7.32</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>7.44</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>7.47</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>7.5750000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5.55</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4.875</v>
+      </c>
+      <c r="L4" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M4" s="3">
+        <v>5.58</v>
+      </c>
+      <c r="N4" s="3">
+        <v>5.97</v>
+      </c>
+      <c r="O4" s="3">
+        <v>7.335</v>
+      </c>
+      <c r="P4" s="3">
+        <v>9.1649999999999991</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>9.57</v>
+      </c>
+      <c r="R4" s="3">
+        <v>10.664999999999999</v>
+      </c>
+      <c r="S4" s="3">
+        <v>11.55</v>
+      </c>
+      <c r="T4" s="3">
+        <v>11.175000000000001</v>
+      </c>
+      <c r="U4" s="3">
+        <v>11.625</v>
+      </c>
+      <c r="V4" s="3">
+        <v>12.404999999999999</v>
+      </c>
+      <c r="W4" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="X4" s="3">
+        <v>12.975</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>13.275</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>14.535</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2.9249999999999998</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.9750000000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.54</v>
+      </c>
+      <c r="G5" s="3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="I5" s="3">
+        <v>5.3250000000000002</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="I6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="J6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="K6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="L6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="M6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="N6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="O6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="P6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="R6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="S6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="T6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="U6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="V6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="W6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="X6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>10.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.255</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="P10" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="U10" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>